<commit_message>
temporary saved AMR updates
</commit_message>
<xml_diff>
--- a/outputs/table_report_for_papers.xlsx
+++ b/outputs/table_report_for_papers.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Table2_epi_all_final_models" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Table1_epi_all_descriptive_perc!$B$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Table1_epi_all_descriptive_perc!$C$3</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Table2_epi_all_final_models!$A$2:$J$10</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="471">
   <si>
     <t xml:space="preserve">Variable</t>
   </si>
@@ -69,7 +69,7 @@
     <t xml:space="preserve">Significance</t>
   </si>
   <si>
-    <t xml:space="preserve">Assessed</t>
+    <t xml:space="preserve">Assessed (n = 450)</t>
   </si>
   <si>
     <r>
@@ -95,6 +95,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Assessed</t>
+  </si>
+  <si>
     <t xml:space="preserve">Study site</t>
   </si>
   <si>
@@ -663,6 +666,9 @@
   </si>
   <si>
     <t xml:space="preserve">0% (0/396)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exclude</t>
   </si>
   <si>
     <t xml:space="preserve">Window type</t>
@@ -1504,7 +1510,7 @@
     <numFmt numFmtId="165" formatCode="0.00"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1540,11 +1546,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1608,7 +1609,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1693,22 +1694,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1717,20 +1702,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1851,117 +1836,115 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K77"/>
+  <dimension ref="A1:L77"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B54" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G17" activeCellId="0" sqref="G17"/>
+      <selection pane="bottomLeft" activeCell="A54" activeCellId="0" sqref="A54"/>
+      <selection pane="bottomRight" activeCell="A76" activeCellId="0" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="36.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="18.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="21.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="18.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="23.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="22.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="17.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="16.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="2" width="11.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="18.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="21.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="18.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="23.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="22.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="17.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="16.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="2" width="11.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4"/>
+      <c r="H1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="6" t="s">
-        <v>5</v>
-      </c>
+      <c r="I1" s="5"/>
       <c r="J1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="6"/>
       <c r="J2" s="6"/>
-      <c r="K2" s="3"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="11" t="s">
+      <c r="K2" s="6"/>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="13" t="n">
+        <v>12</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="13" t="n">
         <v>900</v>
       </c>
-      <c r="H3" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="12"/>
+      <c r="I3" s="14" t="s">
+        <v>15</v>
+      </c>
       <c r="J3" s="12"/>
-      <c r="K3" s="11"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="11"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="12" t="s">
@@ -1976,28 +1959,28 @@
       <c r="F4" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="12" t="s">
         <v>21</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="16" t="n">
+      <c r="I4" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="16" t="n">
         <v>2.51968900957284E-041</v>
-      </c>
-      <c r="J4" s="17" t="s">
-        <v>23</v>
       </c>
       <c r="K4" s="17" t="s">
         <v>24</v>
       </c>
+      <c r="L4" s="17" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15"/>
-      <c r="B5" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="12" t="s">
+      <c r="B5" s="15"/>
+      <c r="C5" s="18" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="12" t="s">
@@ -2009,22 +1992,22 @@
       <c r="F5" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="12" t="s">
         <v>30</v>
       </c>
       <c r="H5" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="16"/>
-      <c r="J5" s="17"/>
+      <c r="I5" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="16"/>
       <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15"/>
-      <c r="B6" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="12" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="18" t="s">
         <v>33</v>
       </c>
       <c r="D6" s="12" t="s">
@@ -2036,21 +2019,21 @@
       <c r="F6" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="12" t="s">
         <v>37</v>
       </c>
       <c r="H6" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="I6" s="16"/>
-      <c r="J6" s="17"/>
+      <c r="I6" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="16"/>
       <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="15" t="s">
         <v>40</v>
       </c>
       <c r="C7" s="12" t="s">
@@ -2065,27 +2048,27 @@
       <c r="F7" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="12" t="s">
         <v>45</v>
       </c>
       <c r="H7" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="I7" s="16" t="n">
+      <c r="I7" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" s="16" t="n">
         <v>0.285978386989364</v>
       </c>
-      <c r="J7" s="16" t="n">
+      <c r="K7" s="16" t="n">
         <v>0.256932122841661</v>
       </c>
-      <c r="K7" s="17" t="s">
-        <v>47</v>
+      <c r="L7" s="17" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15"/>
-      <c r="B8" s="12" t="s">
-        <v>48</v>
-      </c>
+      <c r="B8" s="15"/>
       <c r="C8" s="12" t="s">
         <v>49</v>
       </c>
@@ -2098,21 +2081,21 @@
       <c r="F8" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="12" t="s">
         <v>53</v>
       </c>
       <c r="H8" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="I8" s="16"/>
+      <c r="I8" s="14" t="s">
+        <v>55</v>
+      </c>
       <c r="J8" s="16"/>
-      <c r="K8" s="17"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="17"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="19" t="s">
         <v>56</v>
       </c>
       <c r="C9" s="12" t="s">
@@ -2121,33 +2104,33 @@
       <c r="D9" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="20" t="n">
-        <v>0</v>
+      <c r="E9" s="12" t="s">
+        <v>59</v>
       </c>
       <c r="F9" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="H9" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="I9" s="16" t="n">
+      <c r="J9" s="16" t="n">
         <v>7.18696074084886E-192</v>
-      </c>
-      <c r="J9" s="21" t="s">
-        <v>23</v>
       </c>
       <c r="K9" s="17" t="s">
         <v>24</v>
       </c>
+      <c r="L9" s="17" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="19"/>
-      <c r="B10" s="12" t="s">
-        <v>60</v>
-      </c>
+      <c r="B10" s="19"/>
       <c r="C10" s="12" t="s">
         <v>61</v>
       </c>
@@ -2160,55 +2143,55 @@
       <c r="F10" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="12" t="s">
         <v>65</v>
       </c>
       <c r="H10" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="I10" s="16"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
+      <c r="I10" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="J10" s="16"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="19"/>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="19"/>
+      <c r="C11" s="12" t="s">
         <v>3</v>
-      </c>
-      <c r="C11" s="20" t="n">
-        <v>0</v>
       </c>
       <c r="D11" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="E11" s="12" t="s">
-        <v>67</v>
+      <c r="E11" s="20" t="n">
+        <v>0</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="12" t="s">
         <v>69</v>
       </c>
       <c r="H11" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="J11" s="16"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="12" t="s">
         <v>68</v>
-      </c>
-      <c r="I11" s="16"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>71</v>
       </c>
       <c r="E12" s="12" t="s">
         <v>72</v>
@@ -2216,32 +2199,32 @@
       <c r="F12" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="12" t="s">
         <v>74</v>
       </c>
       <c r="H12" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="I12" s="16" t="n">
+      <c r="I12" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="J12" s="16" t="n">
         <v>0.0151446574453853</v>
       </c>
-      <c r="J12" s="17" t="s">
-        <v>76</v>
-      </c>
       <c r="K12" s="17" t="s">
-        <v>24</v>
+        <v>77</v>
+      </c>
+      <c r="L12" s="17" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="15"/>
-      <c r="B13" s="12" t="s">
-        <v>77</v>
-      </c>
+      <c r="B13" s="15"/>
       <c r="C13" s="12" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="E13" s="12" t="s">
         <v>79</v>
@@ -2249,112 +2232,112 @@
       <c r="F13" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="12" t="s">
         <v>81</v>
       </c>
       <c r="H13" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="I13" s="16"/>
-      <c r="J13" s="17"/>
+      <c r="I13" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="J13" s="16"/>
       <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="22" t="s">
+      <c r="B14" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="C14" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="E14" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="H14" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="I14" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="J14" s="16" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="K14" s="17" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="L14" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="F14" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="G14" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="H14" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="I14" s="16" t="n">
-        <v>0.59</v>
-      </c>
-      <c r="J14" s="17" t="n">
-        <v>0.59</v>
-      </c>
-      <c r="K14" s="17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="D15" s="22" t="s">
+      <c r="C15" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="E15" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="F15" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="G15" s="23" t="s">
+      <c r="G15" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="H15" s="23" t="s">
+      <c r="H15" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="I15" s="16"/>
+      <c r="I15" s="22" t="s">
+        <v>95</v>
+      </c>
       <c r="J15" s="16"/>
-      <c r="K15" s="17"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="17"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="15"/>
-      <c r="B16" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="C16" s="22" t="s">
+      <c r="B16" s="15"/>
+      <c r="C16" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="E16" s="20" t="n">
-        <v>0</v>
+      <c r="E16" s="21" t="s">
+        <v>98</v>
       </c>
       <c r="F16" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="G16" s="23" t="s">
+      <c r="G16" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="I16" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="H16" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="I16" s="16"/>
-      <c r="J16" s="17"/>
+      <c r="J16" s="16"/>
       <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="15" t="s">
         <v>100</v>
       </c>
       <c r="C17" s="12" t="s">
@@ -2369,27 +2352,27 @@
       <c r="F17" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="G17" s="12" t="s">
         <v>105</v>
       </c>
       <c r="H17" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="I17" s="16" t="n">
+      <c r="I17" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="J17" s="16" t="n">
         <v>1.11008246320572E-028</v>
-      </c>
-      <c r="J17" s="17" t="s">
-        <v>23</v>
       </c>
       <c r="K17" s="17" t="s">
         <v>24</v>
       </c>
+      <c r="L17" s="17" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="15"/>
-      <c r="B18" s="12" t="s">
-        <v>107</v>
-      </c>
+      <c r="B18" s="15"/>
       <c r="C18" s="12" t="s">
         <v>108</v>
       </c>
@@ -2402,21 +2385,21 @@
       <c r="F18" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="G18" s="14" t="s">
+      <c r="G18" s="12" t="s">
         <v>112</v>
       </c>
       <c r="H18" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="I18" s="16"/>
-      <c r="J18" s="17"/>
+      <c r="I18" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="J18" s="16"/>
       <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="15"/>
-      <c r="B19" s="12" t="s">
-        <v>114</v>
-      </c>
+      <c r="B19" s="15"/>
       <c r="C19" s="12" t="s">
         <v>115</v>
       </c>
@@ -2429,25 +2412,25 @@
       <c r="F19" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="G19" s="12" t="s">
         <v>119</v>
       </c>
       <c r="H19" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="I19" s="16"/>
-      <c r="J19" s="17"/>
+      <c r="I19" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="J19" s="16"/>
       <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>47</v>
+      <c r="B20" s="15" t="s">
+        <v>122</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>122</v>
+        <v>48</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>123</v>
@@ -2458,29 +2441,29 @@
       <c r="F20" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="12" t="s">
         <v>126</v>
       </c>
       <c r="H20" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="I20" s="16" t="n">
+      <c r="I20" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="J20" s="16" t="n">
         <v>1.10214329180371E-023</v>
-      </c>
-      <c r="J20" s="17" t="s">
-        <v>23</v>
       </c>
       <c r="K20" s="17" t="s">
         <v>24</v>
       </c>
+      <c r="L20" s="17" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="15"/>
-      <c r="B21" s="12" t="s">
-        <v>77</v>
-      </c>
+      <c r="B21" s="15"/>
       <c r="C21" s="12" t="s">
-        <v>128</v>
+        <v>78</v>
       </c>
       <c r="D21" s="12" t="s">
         <v>129</v>
@@ -2491,21 +2474,21 @@
       <c r="F21" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="G21" s="14" t="s">
+      <c r="G21" s="12" t="s">
         <v>132</v>
       </c>
       <c r="H21" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="I21" s="16"/>
-      <c r="J21" s="17"/>
+      <c r="I21" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="J21" s="16"/>
       <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="15" t="s">
         <v>135</v>
       </c>
       <c r="C22" s="12" t="s">
@@ -2520,27 +2503,27 @@
       <c r="F22" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="G22" s="14" t="s">
+      <c r="G22" s="12" t="s">
         <v>140</v>
       </c>
       <c r="H22" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="I22" s="16" t="n">
+      <c r="I22" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="J22" s="16" t="n">
         <v>0.000141417349982951</v>
-      </c>
-      <c r="J22" s="17" t="s">
-        <v>23</v>
       </c>
       <c r="K22" s="17" t="s">
         <v>24</v>
       </c>
+      <c r="L22" s="17" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="15"/>
-      <c r="B23" s="12" t="s">
-        <v>142</v>
-      </c>
+      <c r="B23" s="15"/>
       <c r="C23" s="12" t="s">
         <v>143</v>
       </c>
@@ -2553,48 +2536,48 @@
       <c r="F23" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="G23" s="14" t="s">
+      <c r="G23" s="12" t="s">
         <v>147</v>
       </c>
       <c r="H23" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="I23" s="16"/>
-      <c r="J23" s="17"/>
+      <c r="I23" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="J23" s="16"/>
       <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="15"/>
-      <c r="B24" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="C24" s="20" t="n">
-        <v>0</v>
+      <c r="B24" s="15"/>
+      <c r="C24" s="12" t="s">
+        <v>150</v>
       </c>
       <c r="D24" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="E24" s="12" t="s">
-        <v>89</v>
+      <c r="E24" s="20" t="n">
+        <v>0</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="G24" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="G24" s="12" t="s">
         <v>151</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="I24" s="16"/>
-      <c r="J24" s="17"/>
+        <v>152</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="J24" s="16"/>
       <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="15" t="s">
         <v>153</v>
       </c>
       <c r="C25" s="12" t="s">
@@ -2609,58 +2592,58 @@
       <c r="F25" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="G25" s="14" t="s">
+      <c r="G25" s="12" t="s">
         <v>158</v>
       </c>
       <c r="H25" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="I25" s="16" t="n">
+      <c r="I25" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="J25" s="16" t="n">
         <v>1.03764504818044E-022</v>
-      </c>
-      <c r="J25" s="17" t="s">
-        <v>23</v>
       </c>
       <c r="K25" s="17" t="s">
         <v>24</v>
       </c>
+      <c r="L25" s="17" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="15"/>
-      <c r="B26" s="12" t="s">
-        <v>160</v>
-      </c>
+      <c r="B26" s="15"/>
       <c r="C26" s="12" t="s">
-        <v>35</v>
+        <v>161</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>161</v>
+        <v>36</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>115</v>
+        <v>162</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="G26" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="G26" s="12" t="s">
         <v>163</v>
       </c>
       <c r="H26" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="I26" s="16"/>
-      <c r="J26" s="17"/>
+      <c r="I26" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="J26" s="16"/>
       <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>47</v>
+      <c r="B27" s="15" t="s">
+        <v>166</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>166</v>
+        <v>48</v>
       </c>
       <c r="D27" s="12" t="s">
         <v>167</v>
@@ -2671,29 +2654,29 @@
       <c r="F27" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="12" t="s">
         <v>170</v>
       </c>
       <c r="H27" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="I27" s="16" t="n">
+      <c r="I27" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="J27" s="16" t="n">
         <v>0.0286779211552422</v>
       </c>
-      <c r="J27" s="17" t="s">
-        <v>76</v>
-      </c>
       <c r="K27" s="17" t="s">
-        <v>24</v>
+        <v>77</v>
+      </c>
+      <c r="L27" s="17" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="15"/>
-      <c r="B28" s="12" t="s">
-        <v>77</v>
-      </c>
+      <c r="B28" s="15"/>
       <c r="C28" s="12" t="s">
-        <v>172</v>
+        <v>78</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>173</v>
@@ -2704,83 +2687,83 @@
       <c r="F28" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="G28" s="14" t="s">
+      <c r="G28" s="12" t="s">
         <v>176</v>
       </c>
       <c r="H28" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="I28" s="16"/>
-      <c r="J28" s="17"/>
+      <c r="I28" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="J28" s="16"/>
       <c r="K28" s="17"/>
+      <c r="L28" s="17"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="19" t="s">
-        <v>178</v>
-      </c>
-      <c r="B29" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" s="25" t="s">
+      <c r="B29" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="D29" s="25" t="s">
+      <c r="C29" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="E29" s="20" t="n">
-        <v>0</v>
+      <c r="E29" s="21" t="s">
+        <v>181</v>
       </c>
       <c r="F29" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="G29" s="26" t="s">
+      <c r="G29" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="I29" s="22" t="s">
         <v>181</v>
       </c>
-      <c r="H29" s="26" t="s">
-        <v>180</v>
-      </c>
-      <c r="I29" s="16" t="n">
+      <c r="J29" s="16" t="n">
         <v>1.83762467204593E-031</v>
-      </c>
-      <c r="J29" s="17" t="s">
-        <v>23</v>
       </c>
       <c r="K29" s="17" t="s">
         <v>24</v>
       </c>
+      <c r="L29" s="17" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="19"/>
-      <c r="B30" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="C30" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="D30" s="25" t="s">
+      <c r="B30" s="19"/>
+      <c r="C30" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="E30" s="25" t="s">
+      <c r="E30" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="F30" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="G30" s="26" t="s">
+      <c r="F30" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="H30" s="26" t="s">
+      <c r="G30" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="H30" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="I30" s="16"/>
-      <c r="J30" s="17"/>
+      <c r="I30" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="J30" s="16"/>
       <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="24" t="s">
         <v>188</v>
       </c>
       <c r="C31" s="12" t="s">
@@ -2795,1526 +2778,1559 @@
       <c r="F31" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="G31" s="14" t="s">
+      <c r="G31" s="12" t="s">
         <v>193</v>
       </c>
       <c r="H31" s="14" t="s">
         <v>194</v>
       </c>
-      <c r="I31" s="16" t="n">
-        <v>0.460106768888285</v>
+      <c r="I31" s="14" t="s">
+        <v>195</v>
       </c>
       <c r="J31" s="16" t="n">
         <v>0.460106768888285</v>
       </c>
-      <c r="K31" s="17" t="s">
-        <v>47</v>
+      <c r="K31" s="16" t="n">
+        <v>0.460106768888285</v>
+      </c>
+      <c r="L31" s="17" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="27"/>
-      <c r="B32" s="12" t="s">
-        <v>195</v>
-      </c>
+      <c r="B32" s="24"/>
       <c r="C32" s="12" t="s">
-        <v>12</v>
+        <v>196</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>196</v>
+        <v>13</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>13</v>
+        <v>197</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="G32" s="14" t="s">
         <v>14</v>
       </c>
+      <c r="G32" s="12" t="s">
+        <v>198</v>
+      </c>
       <c r="H32" s="14" t="s">
-        <v>198</v>
-      </c>
-      <c r="I32" s="16"/>
+        <v>15</v>
+      </c>
+      <c r="I32" s="14" t="s">
+        <v>199</v>
+      </c>
       <c r="J32" s="16"/>
-      <c r="K32" s="17"/>
+      <c r="K32" s="16"/>
+      <c r="L32" s="17"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="15" t="s">
-        <v>199</v>
-      </c>
-      <c r="B33" s="12" t="s">
+      <c r="A33" s="0" t="s">
         <v>200</v>
       </c>
+      <c r="B33" s="15" t="s">
+        <v>201</v>
+      </c>
       <c r="C33" s="12" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="G33" s="14" t="s">
         <v>205</v>
       </c>
+      <c r="G33" s="12" t="s">
+        <v>206</v>
+      </c>
       <c r="H33" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="I33" s="16" t="n">
+        <v>207</v>
+      </c>
+      <c r="I33" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="J33" s="16" t="n">
         <v>2.50586977438301E-032</v>
-      </c>
-      <c r="J33" s="17" t="s">
-        <v>23</v>
       </c>
       <c r="K33" s="17" t="s">
         <v>24</v>
       </c>
+      <c r="L33" s="17" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="15"/>
-      <c r="B34" s="12" t="s">
-        <v>207</v>
-      </c>
+      <c r="A34" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="B34" s="15"/>
       <c r="C34" s="12" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="G34" s="14" t="s">
         <v>212</v>
       </c>
+      <c r="G34" s="12" t="s">
+        <v>213</v>
+      </c>
       <c r="H34" s="14" t="s">
-        <v>213</v>
-      </c>
-      <c r="I34" s="16"/>
-      <c r="J34" s="17"/>
+        <v>214</v>
+      </c>
+      <c r="I34" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="J34" s="16"/>
       <c r="K34" s="17"/>
+      <c r="L34" s="17"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>215</v>
+      <c r="A35" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>216</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>96</v>
+        <v>217</v>
       </c>
       <c r="D35" s="12" t="s">
         <v>97</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>216</v>
+        <v>98</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>217</v>
-      </c>
-      <c r="G35" s="14" t="s">
         <v>218</v>
       </c>
+      <c r="G35" s="12" t="s">
+        <v>219</v>
+      </c>
       <c r="H35" s="14" t="s">
-        <v>219</v>
-      </c>
-      <c r="I35" s="16" t="n">
+        <v>220</v>
+      </c>
+      <c r="I35" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="J35" s="16" t="n">
         <v>7.50087431612977E-058</v>
-      </c>
-      <c r="J35" s="17" t="s">
-        <v>23</v>
       </c>
       <c r="K35" s="17" t="s">
         <v>24</v>
       </c>
+      <c r="L35" s="17" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="15"/>
-      <c r="B36" s="12" t="s">
-        <v>220</v>
-      </c>
+      <c r="A36" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="B36" s="15"/>
       <c r="C36" s="12" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>222</v>
-      </c>
-      <c r="E36" s="20" t="n">
-        <v>0</v>
+        <v>223</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>224</v>
       </c>
       <c r="F36" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="G36" s="14" t="s">
-        <v>163</v>
+      <c r="G36" s="20" t="n">
+        <v>0</v>
       </c>
       <c r="H36" s="14" t="s">
-        <v>222</v>
-      </c>
-      <c r="I36" s="16"/>
-      <c r="J36" s="17"/>
+        <v>164</v>
+      </c>
+      <c r="I36" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="J36" s="16"/>
       <c r="K36" s="17"/>
+      <c r="L36" s="17"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="15"/>
-      <c r="B37" s="12" t="s">
-        <v>223</v>
-      </c>
+      <c r="A37" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="B37" s="15"/>
       <c r="C37" s="12" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="G37" s="14" t="s">
         <v>228</v>
       </c>
+      <c r="G37" s="12" t="s">
+        <v>229</v>
+      </c>
       <c r="H37" s="14" t="s">
-        <v>229</v>
-      </c>
-      <c r="I37" s="16"/>
-      <c r="J37" s="17"/>
+        <v>230</v>
+      </c>
+      <c r="I37" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="J37" s="16"/>
       <c r="K37" s="17"/>
+      <c r="L37" s="17"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="19" t="s">
-        <v>230</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>231</v>
+      <c r="A38" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>232</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>91</v>
+        <v>233</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>232</v>
+        <v>92</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F38" s="12" t="s">
-        <v>234</v>
-      </c>
-      <c r="G38" s="14" t="s">
         <v>235</v>
       </c>
+      <c r="G38" s="12" t="s">
+        <v>236</v>
+      </c>
       <c r="H38" s="14" t="s">
-        <v>236</v>
-      </c>
-      <c r="I38" s="16" t="n">
+        <v>237</v>
+      </c>
+      <c r="I38" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="J38" s="16" t="n">
         <v>1.4877076593695E-016</v>
-      </c>
-      <c r="J38" s="17" t="s">
-        <v>23</v>
       </c>
       <c r="K38" s="17" t="s">
         <v>24</v>
       </c>
+      <c r="L38" s="17" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="19"/>
-      <c r="B39" s="12" t="s">
-        <v>237</v>
-      </c>
+      <c r="A39" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="B39" s="19"/>
       <c r="C39" s="12" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>241</v>
-      </c>
-      <c r="G39" s="14" t="s">
         <v>242</v>
       </c>
+      <c r="G39" s="12" t="s">
+        <v>243</v>
+      </c>
       <c r="H39" s="14" t="s">
-        <v>243</v>
-      </c>
-      <c r="I39" s="16"/>
-      <c r="J39" s="17"/>
+        <v>244</v>
+      </c>
+      <c r="I39" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="J39" s="16"/>
       <c r="K39" s="17"/>
+      <c r="L39" s="17"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="19"/>
-      <c r="B40" s="12" t="s">
-        <v>244</v>
-      </c>
+      <c r="A40" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="B40" s="19"/>
       <c r="C40" s="12" t="s">
-        <v>89</v>
+        <v>246</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="E40" s="20" t="n">
-        <v>0</v>
+        <v>90</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>151</v>
       </c>
       <c r="F40" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="G40" s="14" t="s">
+      <c r="G40" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="I40" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="H40" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="I40" s="16"/>
-      <c r="J40" s="17"/>
+      <c r="J40" s="16"/>
       <c r="K40" s="17"/>
+      <c r="L40" s="17"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="19"/>
-      <c r="B41" s="12" t="s">
-        <v>245</v>
-      </c>
+      <c r="A41" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="B41" s="19"/>
       <c r="C41" s="12" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="F41" s="12" t="s">
-        <v>249</v>
-      </c>
-      <c r="G41" s="14" t="s">
         <v>250</v>
       </c>
+      <c r="G41" s="12" t="s">
+        <v>251</v>
+      </c>
       <c r="H41" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="I41" s="16"/>
-      <c r="J41" s="17"/>
+        <v>252</v>
+      </c>
+      <c r="I41" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="J41" s="16"/>
       <c r="K41" s="17"/>
+      <c r="L41" s="17"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="19"/>
-      <c r="B42" s="12" t="s">
-        <v>252</v>
-      </c>
+      <c r="A42" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="B42" s="19"/>
       <c r="C42" s="12" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F42" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="G42" s="14" t="s">
         <v>257</v>
       </c>
+      <c r="G42" s="12" t="s">
+        <v>258</v>
+      </c>
       <c r="H42" s="14" t="s">
-        <v>258</v>
-      </c>
-      <c r="I42" s="16"/>
-      <c r="J42" s="17"/>
+        <v>259</v>
+      </c>
+      <c r="I42" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="J42" s="16"/>
       <c r="K42" s="17"/>
+      <c r="L42" s="17"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="15" t="s">
-        <v>259</v>
-      </c>
-      <c r="B43" s="12" t="s">
-        <v>47</v>
+      <c r="B43" s="15" t="s">
+        <v>261</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>260</v>
+        <v>48</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>184</v>
+        <v>263</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G43" s="14" t="s">
-        <v>262</v>
+        <v>185</v>
+      </c>
+      <c r="G43" s="12" t="s">
+        <v>14</v>
       </c>
       <c r="H43" s="14" t="s">
-        <v>263</v>
-      </c>
-      <c r="I43" s="16" t="n">
-        <v>0.479011230538846</v>
+        <v>264</v>
+      </c>
+      <c r="I43" s="14" t="s">
+        <v>265</v>
       </c>
       <c r="J43" s="16" t="n">
         <v>0.479011230538846</v>
       </c>
-      <c r="K43" s="17" t="s">
-        <v>47</v>
+      <c r="K43" s="16" t="n">
+        <v>0.479011230538846</v>
+      </c>
+      <c r="L43" s="17" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="15"/>
-      <c r="B44" s="12" t="s">
-        <v>77</v>
-      </c>
+      <c r="B44" s="15"/>
       <c r="C44" s="12" t="s">
-        <v>264</v>
+        <v>78</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>265</v>
-      </c>
-      <c r="E44" s="20" t="n">
-        <v>0</v>
+        <v>266</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>267</v>
       </c>
       <c r="F44" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="G44" s="14" t="s">
-        <v>266</v>
+      <c r="G44" s="20" t="n">
+        <v>0</v>
       </c>
       <c r="H44" s="14" t="s">
-        <v>265</v>
-      </c>
-      <c r="I44" s="16"/>
+        <v>268</v>
+      </c>
+      <c r="I44" s="14" t="s">
+        <v>267</v>
+      </c>
       <c r="J44" s="16"/>
-      <c r="K44" s="17"/>
+      <c r="K44" s="16"/>
+      <c r="L44" s="17"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="15" t="s">
-        <v>267</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>47</v>
+      <c r="B45" s="15" t="s">
+        <v>269</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>166</v>
+        <v>48</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>268</v>
+        <v>167</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="F45" s="12" t="s">
-        <v>270</v>
-      </c>
-      <c r="G45" s="14" t="s">
         <v>271</v>
       </c>
+      <c r="G45" s="12" t="s">
+        <v>272</v>
+      </c>
       <c r="H45" s="14" t="s">
-        <v>272</v>
-      </c>
-      <c r="I45" s="28" t="n">
+        <v>273</v>
+      </c>
+      <c r="I45" s="14" t="s">
+        <v>274</v>
+      </c>
+      <c r="J45" s="25" t="n">
         <v>1.3539926971523E-007</v>
-      </c>
-      <c r="J45" s="17" t="s">
-        <v>23</v>
       </c>
       <c r="K45" s="17" t="s">
         <v>24</v>
       </c>
+      <c r="L45" s="17" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="15"/>
-      <c r="B46" s="12" t="s">
-        <v>77</v>
-      </c>
+      <c r="B46" s="15"/>
       <c r="C46" s="12" t="s">
-        <v>172</v>
+        <v>78</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>273</v>
+        <v>173</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="F46" s="12" t="s">
-        <v>275</v>
-      </c>
-      <c r="G46" s="14" t="s">
         <v>276</v>
       </c>
+      <c r="G46" s="12" t="s">
+        <v>277</v>
+      </c>
       <c r="H46" s="14" t="s">
-        <v>277</v>
-      </c>
-      <c r="I46" s="28"/>
-      <c r="J46" s="17"/>
+        <v>278</v>
+      </c>
+      <c r="I46" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="J46" s="25"/>
       <c r="K46" s="17"/>
+      <c r="L46" s="17"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="15" t="s">
-        <v>278</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>47</v>
+      <c r="B47" s="15" t="s">
+        <v>280</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>279</v>
+        <v>48</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>210</v>
+        <v>282</v>
       </c>
       <c r="F47" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="G47" s="14" t="s">
-        <v>282</v>
+        <v>212</v>
+      </c>
+      <c r="G47" s="12" t="s">
+        <v>283</v>
       </c>
       <c r="H47" s="14" t="s">
-        <v>283</v>
-      </c>
-      <c r="I47" s="28" t="n">
+        <v>284</v>
+      </c>
+      <c r="I47" s="14" t="s">
+        <v>285</v>
+      </c>
+      <c r="J47" s="25" t="n">
         <v>5.0872383E-012</v>
-      </c>
-      <c r="J47" s="17" t="s">
-        <v>23</v>
       </c>
       <c r="K47" s="17" t="s">
         <v>24</v>
       </c>
+      <c r="L47" s="17" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="15"/>
-      <c r="B48" s="12" t="s">
-        <v>77</v>
-      </c>
+      <c r="B48" s="15"/>
       <c r="C48" s="12" t="s">
-        <v>284</v>
+        <v>78</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>203</v>
+        <v>287</v>
       </c>
       <c r="F48" s="12" t="s">
-        <v>286</v>
-      </c>
-      <c r="G48" s="14" t="s">
-        <v>287</v>
+        <v>205</v>
+      </c>
+      <c r="G48" s="12" t="s">
+        <v>288</v>
       </c>
       <c r="H48" s="14" t="s">
-        <v>288</v>
-      </c>
-      <c r="I48" s="28"/>
-      <c r="J48" s="17"/>
+        <v>289</v>
+      </c>
+      <c r="I48" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="J48" s="25"/>
       <c r="K48" s="17"/>
+      <c r="L48" s="17"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="15" t="s">
-        <v>289</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>47</v>
+      <c r="B49" s="15" t="s">
+        <v>291</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>290</v>
+        <v>48</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="F49" s="12" t="s">
-        <v>293</v>
-      </c>
-      <c r="G49" s="14" t="s">
-        <v>147</v>
+        <v>294</v>
+      </c>
+      <c r="G49" s="12" t="s">
+        <v>295</v>
       </c>
       <c r="H49" s="14" t="s">
-        <v>294</v>
-      </c>
-      <c r="I49" s="16" t="n">
-        <v>1</v>
+        <v>148</v>
+      </c>
+      <c r="I49" s="14" t="s">
+        <v>296</v>
       </c>
       <c r="J49" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="K49" s="17" t="s">
-        <v>47</v>
+      <c r="K49" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="L49" s="17" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="15"/>
-      <c r="B50" s="12" t="s">
-        <v>77</v>
-      </c>
+      <c r="B50" s="15"/>
       <c r="C50" s="12" t="s">
-        <v>117</v>
+        <v>78</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>295</v>
+        <v>118</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="F50" s="12" t="s">
-        <v>297</v>
-      </c>
-      <c r="G50" s="14" t="s">
         <v>298</v>
       </c>
+      <c r="G50" s="12" t="s">
+        <v>299</v>
+      </c>
       <c r="H50" s="14" t="s">
-        <v>299</v>
-      </c>
-      <c r="I50" s="16"/>
+        <v>300</v>
+      </c>
+      <c r="I50" s="14" t="s">
+        <v>301</v>
+      </c>
       <c r="J50" s="16"/>
-      <c r="K50" s="17"/>
+      <c r="K50" s="16"/>
+      <c r="L50" s="17"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="19" t="s">
-        <v>300</v>
-      </c>
-      <c r="B51" s="29" t="n">
+      <c r="B51" s="19" t="s">
+        <v>302</v>
+      </c>
+      <c r="C51" s="26" t="n">
         <v>0</v>
       </c>
-      <c r="C51" s="25" t="s">
-        <v>301</v>
-      </c>
-      <c r="D51" s="25" t="s">
-        <v>302</v>
-      </c>
-      <c r="E51" s="25" t="s">
-        <v>290</v>
-      </c>
-      <c r="F51" s="25" t="s">
+      <c r="D51" s="21" t="s">
         <v>303</v>
       </c>
-      <c r="G51" s="26" t="s">
+      <c r="E51" s="21" t="s">
         <v>304</v>
       </c>
-      <c r="H51" s="26" t="s">
+      <c r="F51" s="21" t="s">
+        <v>292</v>
+      </c>
+      <c r="G51" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="I51" s="30" t="n">
+      <c r="H51" s="22" t="s">
+        <v>306</v>
+      </c>
+      <c r="I51" s="22" t="s">
+        <v>307</v>
+      </c>
+      <c r="J51" s="25" t="n">
         <v>0.579729972928839</v>
       </c>
-      <c r="J51" s="30" t="n">
+      <c r="K51" s="25" t="n">
         <v>0.579729972928839</v>
       </c>
-      <c r="K51" s="17" t="s">
-        <v>47</v>
+      <c r="L51" s="17" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="19"/>
-      <c r="B52" s="29" t="n">
+      <c r="B52" s="19"/>
+      <c r="C52" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="C52" s="25" t="s">
-        <v>306</v>
-      </c>
-      <c r="D52" s="25" t="s">
-        <v>307</v>
-      </c>
-      <c r="E52" s="25" t="s">
+      <c r="D52" s="21" t="s">
         <v>308</v>
       </c>
-      <c r="F52" s="25" t="s">
+      <c r="E52" s="21" t="s">
         <v>309</v>
       </c>
-      <c r="G52" s="26" t="s">
+      <c r="F52" s="21" t="s">
         <v>310</v>
       </c>
-      <c r="H52" s="26" t="s">
+      <c r="G52" s="21" t="s">
         <v>311</v>
       </c>
-      <c r="I52" s="30"/>
-      <c r="J52" s="30"/>
-      <c r="K52" s="30"/>
+      <c r="H52" s="22" t="s">
+        <v>312</v>
+      </c>
+      <c r="I52" s="22" t="s">
+        <v>313</v>
+      </c>
+      <c r="J52" s="25"/>
+      <c r="K52" s="25"/>
+      <c r="L52" s="25"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="19"/>
-      <c r="B53" s="29" t="n">
+      <c r="B53" s="19"/>
+      <c r="C53" s="26" t="n">
         <v>2</v>
       </c>
-      <c r="C53" s="25" t="s">
-        <v>312</v>
-      </c>
-      <c r="D53" s="25" t="s">
-        <v>313</v>
-      </c>
-      <c r="E53" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="F53" s="25" t="s">
-        <v>232</v>
-      </c>
-      <c r="G53" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="H53" s="26" t="s">
+      <c r="D53" s="21" t="s">
         <v>314</v>
       </c>
-      <c r="I53" s="30"/>
-      <c r="J53" s="30"/>
-      <c r="K53" s="30"/>
+      <c r="E53" s="21" t="s">
+        <v>315</v>
+      </c>
+      <c r="F53" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="G53" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="H53" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="I53" s="22" t="s">
+        <v>316</v>
+      </c>
+      <c r="J53" s="25"/>
+      <c r="K53" s="25"/>
+      <c r="L53" s="25"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="19"/>
-      <c r="B54" s="29" t="n">
+      <c r="B54" s="19"/>
+      <c r="C54" s="26" t="n">
         <v>3</v>
       </c>
-      <c r="C54" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="D54" s="25" t="s">
-        <v>315</v>
-      </c>
-      <c r="E54" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="F54" s="25" t="s">
+      <c r="D54" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="G54" s="26" t="s">
-        <v>316</v>
-      </c>
-      <c r="H54" s="26" t="s">
+      <c r="E54" s="21" t="s">
         <v>317</v>
       </c>
-      <c r="I54" s="30"/>
-      <c r="J54" s="30"/>
-      <c r="K54" s="30"/>
+      <c r="F54" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="G54" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="H54" s="22" t="s">
+        <v>318</v>
+      </c>
+      <c r="I54" s="22" t="s">
+        <v>319</v>
+      </c>
+      <c r="J54" s="25"/>
+      <c r="K54" s="25"/>
+      <c r="L54" s="25"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="19"/>
-      <c r="B55" s="29" t="n">
+      <c r="B55" s="19"/>
+      <c r="C55" s="26" t="n">
         <v>7</v>
       </c>
-      <c r="C55" s="31" t="n">
+      <c r="D55" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="D55" s="31" t="n">
+      <c r="E55" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="E55" s="25" t="s">
-        <v>264</v>
-      </c>
-      <c r="F55" s="25" t="s">
-        <v>318</v>
-      </c>
-      <c r="G55" s="26" t="s">
+      <c r="F55" s="21" t="s">
         <v>266</v>
       </c>
-      <c r="H55" s="26" t="s">
-        <v>318</v>
-      </c>
-      <c r="I55" s="30"/>
-      <c r="J55" s="30"/>
-      <c r="K55" s="30"/>
+      <c r="G55" s="21" t="s">
+        <v>320</v>
+      </c>
+      <c r="H55" s="22" t="s">
+        <v>268</v>
+      </c>
+      <c r="I55" s="22" t="s">
+        <v>320</v>
+      </c>
+      <c r="J55" s="25"/>
+      <c r="K55" s="25"/>
+      <c r="L55" s="25"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="15" t="s">
-        <v>319</v>
-      </c>
-      <c r="B56" s="12" t="s">
-        <v>47</v>
+      <c r="B56" s="15" t="s">
+        <v>321</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>320</v>
+        <v>48</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="F56" s="12" t="s">
-        <v>323</v>
-      </c>
-      <c r="G56" s="14" t="s">
         <v>324</v>
       </c>
+      <c r="G56" s="12" t="s">
+        <v>325</v>
+      </c>
       <c r="H56" s="14" t="s">
-        <v>325</v>
-      </c>
-      <c r="I56" s="16" t="n">
+        <v>326</v>
+      </c>
+      <c r="I56" s="14" t="s">
+        <v>327</v>
+      </c>
+      <c r="J56" s="16" t="n">
         <v>2.71550557E-012</v>
-      </c>
-      <c r="J56" s="17" t="s">
-        <v>23</v>
       </c>
       <c r="K56" s="17" t="s">
         <v>24</v>
       </c>
+      <c r="L56" s="17" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="15"/>
-      <c r="B57" s="12" t="s">
-        <v>326</v>
-      </c>
+      <c r="B57" s="15"/>
       <c r="C57" s="12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D57" s="12" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F57" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="G57" s="14" t="s">
         <v>331</v>
       </c>
+      <c r="G57" s="12" t="s">
+        <v>332</v>
+      </c>
       <c r="H57" s="14" t="s">
-        <v>332</v>
-      </c>
-      <c r="I57" s="16"/>
-      <c r="J57" s="17"/>
+        <v>333</v>
+      </c>
+      <c r="I57" s="14" t="s">
+        <v>334</v>
+      </c>
+      <c r="J57" s="16"/>
       <c r="K57" s="17"/>
+      <c r="L57" s="17"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="19" t="s">
-        <v>333</v>
-      </c>
-      <c r="B58" s="12" t="n">
+      <c r="B58" s="19" t="s">
+        <v>335</v>
+      </c>
+      <c r="C58" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="C58" s="12" t="s">
-        <v>334</v>
-      </c>
       <c r="D58" s="12" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="F58" s="12" t="s">
-        <v>337</v>
-      </c>
-      <c r="G58" s="14" t="s">
         <v>338</v>
       </c>
+      <c r="G58" s="12" t="s">
+        <v>339</v>
+      </c>
       <c r="H58" s="14" t="s">
-        <v>339</v>
-      </c>
-      <c r="I58" s="16" t="n">
+        <v>340</v>
+      </c>
+      <c r="I58" s="14" t="s">
+        <v>341</v>
+      </c>
+      <c r="J58" s="16" t="n">
         <v>0.000156332196752244</v>
       </c>
-      <c r="J58" s="16" t="s">
-        <v>340</v>
-      </c>
-      <c r="K58" s="17" t="s">
-        <v>47</v>
+      <c r="K58" s="16" t="s">
+        <v>342</v>
+      </c>
+      <c r="L58" s="17" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="19"/>
-      <c r="B59" s="18" t="s">
-        <v>341</v>
-      </c>
-      <c r="C59" s="12" t="s">
-        <v>342</v>
+      <c r="B59" s="19"/>
+      <c r="C59" s="18" t="s">
+        <v>343</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="F59" s="12" t="s">
-        <v>345</v>
-      </c>
-      <c r="G59" s="14" t="s">
         <v>346</v>
       </c>
+      <c r="G59" s="12" t="s">
+        <v>347</v>
+      </c>
       <c r="H59" s="14" t="s">
-        <v>347</v>
-      </c>
-      <c r="I59" s="16"/>
+        <v>348</v>
+      </c>
+      <c r="I59" s="14" t="s">
+        <v>349</v>
+      </c>
       <c r="J59" s="16"/>
-      <c r="K59" s="17"/>
+      <c r="K59" s="16"/>
+      <c r="L59" s="17"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="15" t="s">
-        <v>348</v>
-      </c>
-      <c r="B60" s="12" t="n">
+      <c r="B60" s="15" t="s">
+        <v>350</v>
+      </c>
+      <c r="C60" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="C60" s="12" t="s">
-        <v>168</v>
-      </c>
       <c r="D60" s="12" t="s">
-        <v>349</v>
+        <v>169</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="F60" s="12" t="s">
-        <v>351</v>
-      </c>
-      <c r="G60" s="14" t="s">
         <v>352</v>
       </c>
+      <c r="G60" s="12" t="s">
+        <v>353</v>
+      </c>
       <c r="H60" s="14" t="s">
-        <v>353</v>
-      </c>
-      <c r="I60" s="16" t="n">
+        <v>354</v>
+      </c>
+      <c r="I60" s="14" t="s">
+        <v>355</v>
+      </c>
+      <c r="J60" s="16" t="n">
         <v>1.063492717569E-008</v>
-      </c>
-      <c r="J60" s="17" t="s">
-        <v>23</v>
       </c>
       <c r="K60" s="17" t="s">
         <v>24</v>
       </c>
+      <c r="L60" s="17" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="15"/>
-      <c r="B61" s="18" t="s">
-        <v>354</v>
-      </c>
-      <c r="C61" s="12" t="s">
-        <v>174</v>
+      <c r="B61" s="15"/>
+      <c r="C61" s="18" t="s">
+        <v>356</v>
       </c>
       <c r="D61" s="12" t="s">
-        <v>355</v>
+        <v>175</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="F61" s="12" t="s">
-        <v>357</v>
-      </c>
-      <c r="G61" s="14" t="s">
         <v>358</v>
       </c>
+      <c r="G61" s="12" t="s">
+        <v>359</v>
+      </c>
       <c r="H61" s="14" t="s">
-        <v>359</v>
-      </c>
-      <c r="I61" s="16"/>
-      <c r="J61" s="17"/>
+        <v>360</v>
+      </c>
+      <c r="I61" s="14" t="s">
+        <v>361</v>
+      </c>
+      <c r="J61" s="16"/>
       <c r="K61" s="17"/>
+      <c r="L61" s="17"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="15" t="s">
-        <v>360</v>
-      </c>
-      <c r="B62" s="12" t="s">
-        <v>361</v>
+      <c r="B62" s="15" t="s">
+        <v>362</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>182</v>
+        <v>363</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>362</v>
+        <v>183</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="F62" s="12" t="s">
-        <v>364</v>
-      </c>
-      <c r="G62" s="14" t="s">
         <v>365</v>
       </c>
+      <c r="G62" s="12" t="s">
+        <v>366</v>
+      </c>
       <c r="H62" s="14" t="s">
-        <v>366</v>
-      </c>
-      <c r="I62" s="16" t="n">
+        <v>367</v>
+      </c>
+      <c r="I62" s="14" t="s">
+        <v>368</v>
+      </c>
+      <c r="J62" s="16" t="n">
         <v>4.90515792553714E-018</v>
-      </c>
-      <c r="J62" s="17" t="s">
-        <v>23</v>
       </c>
       <c r="K62" s="17" t="s">
         <v>24</v>
       </c>
+      <c r="L62" s="17" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="15"/>
-      <c r="B63" s="12" t="s">
-        <v>367</v>
-      </c>
+      <c r="B63" s="15"/>
       <c r="C63" s="12" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="E63" s="12" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="F63" s="12" t="s">
-        <v>371</v>
-      </c>
-      <c r="G63" s="14" t="s">
         <v>372</v>
       </c>
+      <c r="G63" s="12" t="s">
+        <v>373</v>
+      </c>
       <c r="H63" s="14" t="s">
-        <v>373</v>
-      </c>
-      <c r="I63" s="16"/>
-      <c r="J63" s="17"/>
+        <v>374</v>
+      </c>
+      <c r="I63" s="14" t="s">
+        <v>375</v>
+      </c>
+      <c r="J63" s="16"/>
       <c r="K63" s="17"/>
+      <c r="L63" s="17"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="15"/>
-      <c r="B64" s="12" t="s">
-        <v>374</v>
-      </c>
+      <c r="B64" s="15"/>
       <c r="C64" s="12" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="D64" s="12" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="F64" s="12" t="s">
-        <v>378</v>
-      </c>
-      <c r="G64" s="14" t="s">
         <v>379</v>
       </c>
+      <c r="G64" s="12" t="s">
+        <v>380</v>
+      </c>
       <c r="H64" s="14" t="s">
-        <v>380</v>
-      </c>
-      <c r="I64" s="16"/>
-      <c r="J64" s="17"/>
+        <v>381</v>
+      </c>
+      <c r="I64" s="14" t="s">
+        <v>382</v>
+      </c>
+      <c r="J64" s="16"/>
       <c r="K64" s="17"/>
+      <c r="L64" s="17"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="15" t="s">
-        <v>381</v>
-      </c>
-      <c r="B65" s="12" t="n">
+      <c r="B65" s="15" t="s">
+        <v>383</v>
+      </c>
+      <c r="C65" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="C65" s="12" t="s">
-        <v>168</v>
-      </c>
       <c r="D65" s="12" t="s">
-        <v>382</v>
+        <v>169</v>
       </c>
       <c r="E65" s="12" t="s">
-        <v>84</v>
+        <v>384</v>
       </c>
       <c r="F65" s="12" t="s">
-        <v>383</v>
-      </c>
-      <c r="G65" s="14" t="s">
-        <v>384</v>
+        <v>85</v>
+      </c>
+      <c r="G65" s="12" t="s">
+        <v>385</v>
       </c>
       <c r="H65" s="14" t="s">
-        <v>385</v>
-      </c>
-      <c r="I65" s="30" t="n">
+        <v>386</v>
+      </c>
+      <c r="I65" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="J65" s="25" t="n">
         <v>0.494215019669608</v>
       </c>
-      <c r="J65" s="30" t="n">
+      <c r="K65" s="25" t="n">
         <v>0.494215019669608</v>
       </c>
-      <c r="K65" s="17" t="s">
-        <v>47</v>
+      <c r="L65" s="17" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="15"/>
-      <c r="B66" s="12" t="n">
+      <c r="B66" s="15"/>
+      <c r="C66" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="C66" s="12" t="s">
-        <v>386</v>
-      </c>
       <c r="D66" s="12" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="E66" s="12" t="s">
-        <v>91</v>
+        <v>389</v>
       </c>
       <c r="F66" s="12" t="s">
-        <v>317</v>
-      </c>
-      <c r="G66" s="14" t="s">
-        <v>388</v>
+        <v>92</v>
+      </c>
+      <c r="G66" s="12" t="s">
+        <v>319</v>
       </c>
       <c r="H66" s="14" t="s">
-        <v>389</v>
-      </c>
-      <c r="I66" s="30"/>
-      <c r="J66" s="30"/>
-      <c r="K66" s="30"/>
+        <v>390</v>
+      </c>
+      <c r="I66" s="14" t="s">
+        <v>391</v>
+      </c>
+      <c r="J66" s="25"/>
+      <c r="K66" s="25"/>
+      <c r="L66" s="25"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="15"/>
-      <c r="B67" s="12" t="n">
+      <c r="B67" s="15"/>
+      <c r="C67" s="12" t="n">
         <v>2</v>
-      </c>
-      <c r="C67" s="12" t="s">
-        <v>96</v>
       </c>
       <c r="D67" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="E67" s="20" t="n">
-        <v>0</v>
+      <c r="E67" s="12" t="s">
+        <v>98</v>
       </c>
       <c r="F67" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="G67" s="14" t="s">
+      <c r="G67" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H67" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="I67" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="H67" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="I67" s="30"/>
-      <c r="J67" s="30"/>
-      <c r="K67" s="30"/>
+      <c r="J67" s="25"/>
+      <c r="K67" s="25"/>
+      <c r="L67" s="25"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="19" t="s">
+      <c r="B68" s="19" t="s">
+        <v>392</v>
+      </c>
+      <c r="C68" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D68" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E68" s="12" t="s">
+        <v>393</v>
+      </c>
+      <c r="F68" s="12" t="s">
+        <v>394</v>
+      </c>
+      <c r="G68" s="12" t="s">
+        <v>395</v>
+      </c>
+      <c r="H68" s="14" t="s">
+        <v>396</v>
+      </c>
+      <c r="I68" s="14" t="s">
+        <v>397</v>
+      </c>
+      <c r="J68" s="25" t="n">
+        <v>0.672687913339049</v>
+      </c>
+      <c r="K68" s="25" t="n">
+        <v>0.672687913339049</v>
+      </c>
+      <c r="L68" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B69" s="19"/>
+      <c r="C69" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D69" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="E69" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="F69" s="12" t="s">
+        <v>388</v>
+      </c>
+      <c r="G69" s="12" t="s">
+        <v>398</v>
+      </c>
+      <c r="H69" s="14" t="s">
         <v>390</v>
       </c>
-      <c r="B68" s="12" t="n">
+      <c r="I69" s="14" t="s">
+        <v>399</v>
+      </c>
+      <c r="J69" s="25"/>
+      <c r="K69" s="25"/>
+      <c r="L69" s="25"/>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B70" s="19" t="s">
+        <v>400</v>
+      </c>
+      <c r="C70" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="C68" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D68" s="12" t="s">
-        <v>391</v>
-      </c>
-      <c r="E68" s="12" t="s">
-        <v>392</v>
-      </c>
-      <c r="F68" s="12" t="s">
-        <v>393</v>
-      </c>
-      <c r="G68" s="14" t="s">
-        <v>394</v>
-      </c>
-      <c r="H68" s="14" t="s">
-        <v>395</v>
-      </c>
-      <c r="I68" s="30" t="n">
-        <v>0.672687913339049</v>
-      </c>
-      <c r="J68" s="30" t="n">
-        <v>0.672687913339049</v>
-      </c>
-      <c r="K68" s="17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="19"/>
-      <c r="B69" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="C69" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="D69" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="E69" s="12" t="s">
-        <v>386</v>
-      </c>
-      <c r="F69" s="12" t="s">
-        <v>396</v>
-      </c>
-      <c r="G69" s="14" t="s">
-        <v>388</v>
-      </c>
-      <c r="H69" s="14" t="s">
-        <v>397</v>
-      </c>
-      <c r="I69" s="30"/>
-      <c r="J69" s="30"/>
-      <c r="K69" s="30"/>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="19" t="s">
-        <v>398</v>
-      </c>
-      <c r="B70" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="C70" s="12" t="s">
-        <v>399</v>
-      </c>
       <c r="D70" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="E70" s="12" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="F70" s="12" t="s">
-        <v>402</v>
-      </c>
-      <c r="G70" s="14" t="s">
         <v>403</v>
       </c>
+      <c r="G70" s="12" t="s">
+        <v>404</v>
+      </c>
       <c r="H70" s="14" t="s">
-        <v>404</v>
-      </c>
-      <c r="I70" s="30" t="n">
+        <v>405</v>
+      </c>
+      <c r="I70" s="14" t="s">
+        <v>406</v>
+      </c>
+      <c r="J70" s="25" t="n">
         <v>3.7465208641593E-007</v>
-      </c>
-      <c r="J70" s="17" t="s">
-        <v>23</v>
       </c>
       <c r="K70" s="17" t="s">
         <v>24</v>
       </c>
+      <c r="L70" s="17" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="19"/>
-      <c r="B71" s="12" t="n">
+      <c r="B71" s="19"/>
+      <c r="C71" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="C71" s="12" t="s">
-        <v>405</v>
-      </c>
       <c r="D71" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="E71" s="12" t="s">
-        <v>356</v>
+        <v>408</v>
       </c>
       <c r="F71" s="12" t="s">
-        <v>407</v>
-      </c>
-      <c r="G71" s="14" t="s">
-        <v>408</v>
+        <v>358</v>
+      </c>
+      <c r="G71" s="12" t="s">
+        <v>409</v>
       </c>
       <c r="H71" s="14" t="s">
-        <v>409</v>
-      </c>
-      <c r="I71" s="30"/>
-      <c r="J71" s="30"/>
-      <c r="K71" s="30"/>
+        <v>410</v>
+      </c>
+      <c r="I71" s="14" t="s">
+        <v>411</v>
+      </c>
+      <c r="J71" s="25"/>
+      <c r="K71" s="25"/>
+      <c r="L71" s="25"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="19"/>
-      <c r="B72" s="12" t="n">
+      <c r="B72" s="19"/>
+      <c r="C72" s="12" t="n">
         <v>2</v>
-      </c>
-      <c r="C72" s="20" t="n">
-        <v>0</v>
       </c>
       <c r="D72" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="E72" s="12" t="s">
-        <v>63</v>
+      <c r="E72" s="20" t="n">
+        <v>0</v>
       </c>
       <c r="F72" s="12" t="s">
-        <v>410</v>
-      </c>
-      <c r="G72" s="14" t="s">
-        <v>411</v>
+        <v>64</v>
+      </c>
+      <c r="G72" s="12" t="s">
+        <v>412</v>
       </c>
       <c r="H72" s="14" t="s">
-        <v>410</v>
-      </c>
-      <c r="I72" s="30"/>
-      <c r="J72" s="30"/>
-      <c r="K72" s="30"/>
+        <v>413</v>
+      </c>
+      <c r="I72" s="14" t="s">
+        <v>412</v>
+      </c>
+      <c r="J72" s="25"/>
+      <c r="K72" s="25"/>
+      <c r="L72" s="25"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="19"/>
-      <c r="B73" s="12" t="n">
+      <c r="B73" s="19"/>
+      <c r="C73" s="12" t="n">
         <v>3</v>
-      </c>
-      <c r="C73" s="20" t="n">
-        <v>0</v>
       </c>
       <c r="D73" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="E73" s="12" t="s">
-        <v>96</v>
+      <c r="E73" s="20" t="n">
+        <v>0</v>
       </c>
       <c r="F73" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="G73" s="14" t="s">
+      <c r="G73" s="12" t="s">
         <v>98</v>
       </c>
       <c r="H73" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="I73" s="30"/>
-      <c r="J73" s="30"/>
-      <c r="K73" s="30"/>
+        <v>99</v>
+      </c>
+      <c r="I73" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="J73" s="25"/>
+      <c r="K73" s="25"/>
+      <c r="L73" s="25"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="15" t="s">
-        <v>412</v>
-      </c>
-      <c r="B74" s="12" t="s">
-        <v>413</v>
+      <c r="B74" s="15" t="s">
+        <v>414</v>
       </c>
       <c r="C74" s="12" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D74" s="12" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="E74" s="12" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F74" s="12" t="s">
-        <v>417</v>
-      </c>
-      <c r="G74" s="14" t="s">
         <v>418</v>
       </c>
+      <c r="G74" s="12" t="s">
+        <v>419</v>
+      </c>
       <c r="H74" s="14" t="s">
-        <v>419</v>
-      </c>
-      <c r="I74" s="16" t="n">
+        <v>420</v>
+      </c>
+      <c r="I74" s="14" t="s">
+        <v>421</v>
+      </c>
+      <c r="J74" s="16" t="n">
         <v>2.926715E-014</v>
-      </c>
-      <c r="J74" s="17" t="s">
-        <v>23</v>
       </c>
       <c r="K74" s="17" t="s">
         <v>24</v>
       </c>
+      <c r="L74" s="17" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="15"/>
-      <c r="B75" s="12" t="s">
-        <v>420</v>
-      </c>
+      <c r="B75" s="15"/>
       <c r="C75" s="12" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="D75" s="12" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="E75" s="12" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="F75" s="12" t="s">
-        <v>424</v>
-      </c>
-      <c r="G75" s="14" t="s">
         <v>425</v>
       </c>
+      <c r="G75" s="12" t="s">
+        <v>426</v>
+      </c>
       <c r="H75" s="14" t="s">
-        <v>426</v>
-      </c>
-      <c r="I75" s="16"/>
-      <c r="J75" s="17"/>
+        <v>427</v>
+      </c>
+      <c r="I75" s="14" t="s">
+        <v>428</v>
+      </c>
+      <c r="J75" s="16"/>
       <c r="K75" s="17"/>
+      <c r="L75" s="17"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="15" t="s">
-        <v>427</v>
-      </c>
-      <c r="B76" s="12" t="s">
-        <v>428</v>
+      <c r="B76" s="15" t="s">
+        <v>429</v>
       </c>
       <c r="C76" s="12" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="D76" s="12" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="E76" s="12" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="F76" s="12" t="s">
-        <v>432</v>
-      </c>
-      <c r="G76" s="14" t="s">
         <v>433</v>
       </c>
+      <c r="G76" s="12" t="s">
+        <v>434</v>
+      </c>
       <c r="H76" s="14" t="s">
-        <v>434</v>
-      </c>
-      <c r="I76" s="16" t="n">
+        <v>435</v>
+      </c>
+      <c r="I76" s="14" t="s">
+        <v>436</v>
+      </c>
+      <c r="J76" s="16" t="n">
         <v>0.041683818853692</v>
       </c>
-      <c r="J76" s="17" t="s">
-        <v>76</v>
-      </c>
       <c r="K76" s="17" t="s">
-        <v>24</v>
+        <v>77</v>
+      </c>
+      <c r="L76" s="17" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="15"/>
-      <c r="B77" s="12" t="s">
-        <v>435</v>
-      </c>
+      <c r="B77" s="15"/>
       <c r="C77" s="12" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="D77" s="12" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="E77" s="12" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="F77" s="12" t="s">
-        <v>439</v>
-      </c>
-      <c r="G77" s="14" t="s">
         <v>440</v>
       </c>
+      <c r="G77" s="12" t="s">
+        <v>441</v>
+      </c>
       <c r="H77" s="14" t="s">
-        <v>441</v>
-      </c>
-      <c r="I77" s="16"/>
-      <c r="J77" s="17"/>
+        <v>442</v>
+      </c>
+      <c r="I77" s="14" t="s">
+        <v>443</v>
+      </c>
+      <c r="J77" s="16"/>
       <c r="K77" s="17"/>
+      <c r="L77" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="124">
-    <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="I4:I6"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="B4:B6"/>
     <mergeCell ref="J4:J6"/>
     <mergeCell ref="K4:K6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="B7:B8"/>
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="K7:K8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="B9:B11"/>
     <mergeCell ref="J9:J11"/>
     <mergeCell ref="K9:K11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="L9:L11"/>
+    <mergeCell ref="B12:B13"/>
     <mergeCell ref="J12:J13"/>
     <mergeCell ref="K12:K13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="I14:I16"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="B14:B16"/>
     <mergeCell ref="J14:J16"/>
     <mergeCell ref="K14:K16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="I17:I19"/>
+    <mergeCell ref="L14:L16"/>
+    <mergeCell ref="B17:B19"/>
     <mergeCell ref="J17:J19"/>
     <mergeCell ref="K17:K19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="L17:L19"/>
+    <mergeCell ref="B20:B21"/>
     <mergeCell ref="J20:J21"/>
     <mergeCell ref="K20:K21"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="I22:I24"/>
+    <mergeCell ref="L20:L21"/>
+    <mergeCell ref="B22:B24"/>
     <mergeCell ref="J22:J24"/>
     <mergeCell ref="K22:K24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="I25:I26"/>
+    <mergeCell ref="L22:L24"/>
+    <mergeCell ref="B25:B26"/>
     <mergeCell ref="J25:J26"/>
     <mergeCell ref="K25:K26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="L25:L26"/>
+    <mergeCell ref="B27:B28"/>
     <mergeCell ref="J27:J28"/>
     <mergeCell ref="K27:K28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="I29:I30"/>
+    <mergeCell ref="L27:L28"/>
+    <mergeCell ref="B29:B30"/>
     <mergeCell ref="J29:J30"/>
     <mergeCell ref="K29:K30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="I31:I32"/>
+    <mergeCell ref="L29:L30"/>
+    <mergeCell ref="B31:B32"/>
     <mergeCell ref="J31:J32"/>
     <mergeCell ref="K31:K32"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="L31:L32"/>
+    <mergeCell ref="B33:B34"/>
     <mergeCell ref="J33:J34"/>
     <mergeCell ref="K33:K34"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="I35:I37"/>
+    <mergeCell ref="L33:L34"/>
+    <mergeCell ref="B35:B37"/>
     <mergeCell ref="J35:J37"/>
     <mergeCell ref="K35:K37"/>
-    <mergeCell ref="A38:A42"/>
-    <mergeCell ref="I38:I42"/>
+    <mergeCell ref="L35:L37"/>
+    <mergeCell ref="B38:B42"/>
     <mergeCell ref="J38:J42"/>
     <mergeCell ref="K38:K42"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="I43:I44"/>
+    <mergeCell ref="L38:L42"/>
+    <mergeCell ref="B43:B44"/>
     <mergeCell ref="J43:J44"/>
     <mergeCell ref="K43:K44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="I45:I46"/>
+    <mergeCell ref="L43:L44"/>
+    <mergeCell ref="B45:B46"/>
     <mergeCell ref="J45:J46"/>
     <mergeCell ref="K45:K46"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="I47:I48"/>
+    <mergeCell ref="L45:L46"/>
+    <mergeCell ref="B47:B48"/>
     <mergeCell ref="J47:J48"/>
     <mergeCell ref="K47:K48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="I49:I50"/>
+    <mergeCell ref="L47:L48"/>
+    <mergeCell ref="B49:B50"/>
     <mergeCell ref="J49:J50"/>
     <mergeCell ref="K49:K50"/>
-    <mergeCell ref="A51:A55"/>
-    <mergeCell ref="I51:I55"/>
+    <mergeCell ref="L49:L50"/>
+    <mergeCell ref="B51:B55"/>
     <mergeCell ref="J51:J55"/>
     <mergeCell ref="K51:K55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="I56:I57"/>
+    <mergeCell ref="L51:L55"/>
+    <mergeCell ref="B56:B57"/>
     <mergeCell ref="J56:J57"/>
     <mergeCell ref="K56:K57"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="I58:I59"/>
+    <mergeCell ref="L56:L57"/>
+    <mergeCell ref="B58:B59"/>
     <mergeCell ref="J58:J59"/>
     <mergeCell ref="K58:K59"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="I60:I61"/>
+    <mergeCell ref="L58:L59"/>
+    <mergeCell ref="B60:B61"/>
     <mergeCell ref="J60:J61"/>
     <mergeCell ref="K60:K61"/>
-    <mergeCell ref="A62:A64"/>
-    <mergeCell ref="I62:I64"/>
+    <mergeCell ref="L60:L61"/>
+    <mergeCell ref="B62:B64"/>
     <mergeCell ref="J62:J64"/>
     <mergeCell ref="K62:K64"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="I65:I67"/>
+    <mergeCell ref="L62:L64"/>
+    <mergeCell ref="B65:B67"/>
     <mergeCell ref="J65:J67"/>
     <mergeCell ref="K65:K67"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="I68:I69"/>
+    <mergeCell ref="L65:L67"/>
+    <mergeCell ref="B68:B69"/>
     <mergeCell ref="J68:J69"/>
     <mergeCell ref="K68:K69"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="I70:I73"/>
+    <mergeCell ref="L68:L69"/>
+    <mergeCell ref="B70:B73"/>
     <mergeCell ref="J70:J73"/>
     <mergeCell ref="K70:K73"/>
-    <mergeCell ref="A74:A75"/>
-    <mergeCell ref="I74:I75"/>
+    <mergeCell ref="L70:L73"/>
+    <mergeCell ref="B74:B75"/>
     <mergeCell ref="J74:J75"/>
     <mergeCell ref="K74:K75"/>
-    <mergeCell ref="A76:A77"/>
-    <mergeCell ref="I76:I77"/>
+    <mergeCell ref="L74:L75"/>
+    <mergeCell ref="B76:B77"/>
     <mergeCell ref="J76:J77"/>
     <mergeCell ref="K76:K77"/>
+    <mergeCell ref="L76:L77"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -4351,7 +4367,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="5.06"/>
   </cols>
   <sheetData>
-    <row r="1" s="32" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="28" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4359,326 +4375,326 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
     </row>
-    <row r="2" s="32" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="28" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="33" t="s">
-        <v>445</v>
-      </c>
-      <c r="D2" s="34" t="s">
-        <v>446</v>
-      </c>
-      <c r="E2" s="34" t="s">
-        <v>446</v>
-      </c>
-      <c r="F2" s="33" t="s">
-        <v>445</v>
-      </c>
-      <c r="G2" s="34" t="s">
-        <v>446</v>
-      </c>
-      <c r="H2" s="34" t="s">
-        <v>446</v>
-      </c>
-      <c r="I2" s="33" t="s">
-        <v>445</v>
-      </c>
-      <c r="J2" s="34" t="s">
-        <v>446</v>
-      </c>
-      <c r="K2" s="34" t="s">
-        <v>446</v>
+      <c r="C2" s="29" t="s">
+        <v>447</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>448</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>448</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>447</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>448</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>448</v>
+      </c>
+      <c r="I2" s="29" t="s">
+        <v>447</v>
+      </c>
+      <c r="J2" s="30" t="s">
+        <v>448</v>
+      </c>
+      <c r="K2" s="30" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
-        <v>178</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>447</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>448</v>
-      </c>
-      <c r="D3" s="35" t="n">
+        <v>179</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>449</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>450</v>
+      </c>
+      <c r="D3" s="31" t="n">
         <v>0.999999999999992</v>
       </c>
-      <c r="E3" s="35" t="n">
+      <c r="E3" s="31" t="n">
         <v>0.999999999999992</v>
       </c>
-      <c r="F3" s="25" t="s">
-        <v>449</v>
-      </c>
-      <c r="G3" s="36" t="n">
+      <c r="F3" s="21" t="s">
+        <v>451</v>
+      </c>
+      <c r="G3" s="32" t="n">
         <v>0.303441147154513</v>
       </c>
-      <c r="H3" s="36" t="n">
+      <c r="H3" s="32" t="n">
         <v>0.303441147154513</v>
       </c>
-      <c r="I3" s="25" t="s">
-        <v>450</v>
-      </c>
-      <c r="J3" s="36" t="n">
+      <c r="I3" s="21" t="s">
+        <v>452</v>
+      </c>
+      <c r="J3" s="32" t="n">
         <v>0.568402560924381</v>
       </c>
-      <c r="K3" s="36" t="n">
+      <c r="K3" s="32" t="n">
         <v>0.568402560924381</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19"/>
-      <c r="B4" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>451</v>
-      </c>
-      <c r="D4" s="35" t="n">
+      <c r="B4" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>453</v>
+      </c>
+      <c r="D4" s="31" t="n">
         <v>0.155806680571467</v>
       </c>
-      <c r="E4" s="35" t="n">
+      <c r="E4" s="31" t="n">
         <v>0.155806680571467</v>
       </c>
-      <c r="F4" s="25" t="s">
-        <v>452</v>
-      </c>
-      <c r="G4" s="36" t="n">
+      <c r="F4" s="21" t="s">
+        <v>454</v>
+      </c>
+      <c r="G4" s="32" t="n">
         <v>0.0394109353506562</v>
       </c>
-      <c r="H4" s="36" t="s">
-        <v>453</v>
-      </c>
-      <c r="I4" s="25" t="s">
-        <v>454</v>
-      </c>
-      <c r="J4" s="36" t="n">
+      <c r="H4" s="32" t="s">
+        <v>455</v>
+      </c>
+      <c r="I4" s="21" t="s">
+        <v>456</v>
+      </c>
+      <c r="J4" s="32" t="n">
         <v>0.0855167983975968</v>
       </c>
-      <c r="K4" s="36" t="n">
+      <c r="K4" s="32" t="n">
         <v>0.0855167983975968</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>267</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>447</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>455</v>
-      </c>
-      <c r="D5" s="35" t="n">
+        <v>269</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>449</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>457</v>
+      </c>
+      <c r="D5" s="31" t="n">
         <v>0.000255745624885517</v>
       </c>
-      <c r="E5" s="35" t="s">
-        <v>340</v>
-      </c>
-      <c r="F5" s="25" t="s">
-        <v>449</v>
-      </c>
-      <c r="G5" s="36" t="n">
+      <c r="E5" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>451</v>
+      </c>
+      <c r="G5" s="32" t="n">
         <v>0.303441147154513</v>
       </c>
-      <c r="H5" s="36" t="n">
+      <c r="H5" s="32" t="n">
         <v>0.303441147154513</v>
       </c>
-      <c r="I5" s="25" t="s">
-        <v>450</v>
-      </c>
-      <c r="J5" s="36" t="n">
+      <c r="I5" s="21" t="s">
+        <v>452</v>
+      </c>
+      <c r="J5" s="32" t="n">
         <v>0.568402560924381</v>
       </c>
-      <c r="K5" s="36" t="n">
+      <c r="K5" s="32" t="n">
         <v>0.568402560924381</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="15"/>
-      <c r="B6" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>456</v>
-      </c>
-      <c r="D6" s="35" t="n">
+      <c r="B6" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>458</v>
+      </c>
+      <c r="D6" s="31" t="n">
         <v>0.395964289961191</v>
       </c>
-      <c r="E6" s="35" t="n">
+      <c r="E6" s="31" t="n">
         <v>0.395964289961191</v>
       </c>
-      <c r="F6" s="25" t="s">
-        <v>457</v>
-      </c>
-      <c r="G6" s="36" t="n">
+      <c r="F6" s="21" t="s">
+        <v>459</v>
+      </c>
+      <c r="G6" s="32" t="n">
         <v>0.0599481021236772</v>
       </c>
-      <c r="H6" s="36" t="n">
+      <c r="H6" s="32" t="n">
         <v>0.0599481021236772</v>
       </c>
-      <c r="I6" s="25" t="s">
-        <v>458</v>
-      </c>
-      <c r="J6" s="36" t="n">
+      <c r="I6" s="21" t="s">
+        <v>460</v>
+      </c>
+      <c r="J6" s="32" t="n">
         <v>0.133397958911203</v>
       </c>
-      <c r="K6" s="36" t="n">
+      <c r="K6" s="32" t="n">
         <v>0.133397958911203</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="15" t="s">
-        <v>319</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>447</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>459</v>
-      </c>
-      <c r="D7" s="35" t="n">
+        <v>321</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>449</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>461</v>
+      </c>
+      <c r="D7" s="31" t="n">
         <v>1.54876268746972E-006</v>
       </c>
-      <c r="E7" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="25" t="s">
-        <v>449</v>
-      </c>
-      <c r="G7" s="36" t="n">
+      <c r="E7" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>451</v>
+      </c>
+      <c r="G7" s="32" t="n">
         <v>0.303441147154513</v>
       </c>
-      <c r="H7" s="36" t="n">
+      <c r="H7" s="32" t="n">
         <v>0.303441147154513</v>
       </c>
-      <c r="I7" s="25" t="s">
-        <v>450</v>
-      </c>
-      <c r="J7" s="36" t="n">
+      <c r="I7" s="21" t="s">
+        <v>452</v>
+      </c>
+      <c r="J7" s="32" t="n">
         <v>0.568402560924381</v>
       </c>
-      <c r="K7" s="36" t="n">
+      <c r="K7" s="32" t="n">
         <v>0.568402560924381</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="15"/>
-      <c r="B8" s="25" t="s">
-        <v>326</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>460</v>
-      </c>
-      <c r="D8" s="35" t="n">
+      <c r="B8" s="21" t="s">
+        <v>328</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>462</v>
+      </c>
+      <c r="D8" s="31" t="n">
         <v>0.000684997333219925</v>
       </c>
-      <c r="E8" s="35" t="s">
-        <v>340</v>
-      </c>
-      <c r="F8" s="25" t="s">
-        <v>461</v>
-      </c>
-      <c r="G8" s="36" t="n">
+      <c r="E8" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>463</v>
+      </c>
+      <c r="G8" s="32" t="n">
         <v>0.057030481435603</v>
       </c>
-      <c r="H8" s="36" t="n">
+      <c r="H8" s="32" t="n">
         <v>0.057030481435603</v>
       </c>
-      <c r="I8" s="25" t="s">
-        <v>462</v>
-      </c>
-      <c r="J8" s="36" t="n">
+      <c r="I8" s="21" t="s">
+        <v>464</v>
+      </c>
+      <c r="J8" s="32" t="n">
         <v>0.000270137478692095</v>
       </c>
-      <c r="K8" s="35" t="s">
-        <v>340</v>
+      <c r="K8" s="31" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="15" t="s">
-        <v>381</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>463</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>464</v>
-      </c>
-      <c r="D9" s="35" t="n">
+        <v>383</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>465</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>466</v>
+      </c>
+      <c r="D9" s="31" t="n">
         <v>0.00014849670750264</v>
       </c>
-      <c r="E9" s="35" t="s">
-        <v>340</v>
-      </c>
-      <c r="F9" s="25" t="s">
-        <v>449</v>
-      </c>
-      <c r="G9" s="36" t="n">
+      <c r="E9" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>451</v>
+      </c>
+      <c r="G9" s="32" t="n">
         <v>0.303441147154513</v>
       </c>
-      <c r="H9" s="36" t="n">
+      <c r="H9" s="32" t="n">
         <v>0.303441147154513</v>
       </c>
-      <c r="I9" s="25" t="s">
-        <v>450</v>
-      </c>
-      <c r="J9" s="36" t="n">
+      <c r="I9" s="21" t="s">
+        <v>452</v>
+      </c>
+      <c r="J9" s="32" t="n">
         <v>0.568402560924381</v>
       </c>
-      <c r="K9" s="36" t="n">
+      <c r="K9" s="32" t="n">
         <v>0.568402560924381</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="15"/>
-      <c r="B10" s="25" t="s">
-        <v>465</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>466</v>
-      </c>
-      <c r="D10" s="35" t="n">
+      <c r="B10" s="21" t="s">
+        <v>467</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>468</v>
+      </c>
+      <c r="D10" s="31" t="n">
         <v>0.123718478645134</v>
       </c>
-      <c r="E10" s="35" t="n">
+      <c r="E10" s="31" t="n">
         <v>0.123718478645134</v>
       </c>
-      <c r="F10" s="25" t="s">
-        <v>467</v>
-      </c>
-      <c r="G10" s="36" t="n">
+      <c r="F10" s="21" t="s">
+        <v>469</v>
+      </c>
+      <c r="G10" s="32" t="n">
         <v>0.0609612032808228</v>
       </c>
-      <c r="H10" s="36" t="n">
+      <c r="H10" s="32" t="n">
         <v>0.0609612032808228</v>
       </c>
-      <c r="I10" s="25" t="s">
-        <v>468</v>
-      </c>
-      <c r="J10" s="36" t="n">
+      <c r="I10" s="21" t="s">
+        <v>470</v>
+      </c>
+      <c r="J10" s="32" t="n">
         <v>0.15576820805247</v>
       </c>
-      <c r="K10" s="36" t="n">
+      <c r="K10" s="32" t="n">
         <v>0.15576820805247</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="37"/>
+      <c r="A11" s="33"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:J10"/>

</xml_diff>